<commit_message>
Create Alumni, and change the tagihan method
</commit_message>
<xml_diff>
--- a/public/assets/download/document/simpanan.xlsx
+++ b/public/assets/download/document/simpanan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>No</t>
   </si>
@@ -41,10 +41,7 @@
     <t>Tagihan</t>
   </si>
   <si>
-    <t>Bakda Pratiwi</t>
-  </si>
-  <si>
-    <t>2083/Kopma_UL/21</t>
+    <t>2083/Kopma_Ul/21</t>
   </si>
   <si>
     <t>Anggota</t>
@@ -57,6 +54,15 @@
   </si>
   <si>
     <t>Anggota Luar Biasa</t>
+  </si>
+  <si>
+    <t>Rian</t>
+  </si>
+  <si>
+    <t>2086/Kopma_UL/20</t>
+  </si>
+  <si>
+    <t>-- Status Keanggotaan --</t>
   </si>
   <si>
     <t>Hartana Prima Prayoga S.Kom</t>
@@ -440,7 +446,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,14 +484,12 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2"/>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>30000</v>
@@ -497,7 +501,7 @@
         <v>70000</v>
       </c>
       <c r="H2">
-        <v>80000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -505,25 +509,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
       <c r="E3">
         <v>30000</v>
       </c>
       <c r="F3">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="G3">
-        <v>80000</v>
+        <v>60000</v>
       </c>
       <c r="H3">
-        <v>70000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -531,23 +535,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4"/>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>-15000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -565,13 +571,13 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>50000</v>
+        <v>150000</v>
       </c>
       <c r="G5">
-        <v>50000</v>
+        <v>150000</v>
       </c>
       <c r="H5">
-        <v>85000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -589,13 +595,13 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="H6">
-        <v>135000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -619,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>135000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -643,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>135000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -667,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>135000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -691,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>135000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -715,7 +721,31 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>135000</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>